<commit_message>
updated hotel instructions. no payment
</commit_message>
<xml_diff>
--- a/docs/2023RSS-RoomReservationRequestForm.xlsx
+++ b/docs/2023RSS-RoomReservationRequestForm.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Request Form'!$A$1:$E$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Request Form'!$A$1:$E$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Room Type</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Credit Card Information</t>
   </si>
   <si>
     <t>Guest
@@ -132,27 +129,6 @@
   </si>
   <si>
     <t>Number of Night</t>
-  </si>
-  <si>
-    <t>Name as it appears on the card</t>
-  </si>
-  <si>
-    <t>CARDHOLDER INFORMATION - Required</t>
-  </si>
-  <si>
-    <t>(ex. VISA, Master, Amex, etc.)</t>
-  </si>
-  <si>
-    <t>Crad Type</t>
-  </si>
-  <si>
-    <t>Issuing Bank</t>
-  </si>
-  <si>
-    <t>Card Number</t>
-  </si>
-  <si>
-    <t>Expiry Date</t>
   </si>
   <si>
     <t>Guest Name</t>
@@ -264,6 +240,22 @@
     <t>Saturday
  (Jul. 08, 2023)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reservation Guarantee
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Once your reservation request is processed, a secured link for credit card information will be sent to your email. Upon receiving your credit card information for guarantee through the Marriott's secured system, your room reservation confirmation which will prove and finally confirm your room reservation will be sent via email. </t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -289,15 +281,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -344,6 +327,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -774,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -835,7 +825,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,35 +834,41 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -883,6 +878,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -970,15 +969,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1343,10 +1347,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:D44"/>
+      <selection activeCell="A28" sqref="A28:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1359,136 +1363,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1">
-      <c r="A1" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="A1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="23.25" customHeight="1">
+      <c r="A12" s="40"/>
+      <c r="B12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A12" s="38"/>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="43"/>
+    </row>
+    <row r="13" spans="1:5" ht="23.25" customHeight="1">
+      <c r="A13" s="40"/>
+      <c r="B13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A13" s="38"/>
-      <c r="B13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="43"/>
     </row>
     <row r="14" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A14" s="38"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A15" s="39"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="64">
+        <v>30</v>
+      </c>
+      <c r="C15" s="24">
         <f>IF((E14-C14)&lt;0,0,E14-C14)</f>
         <v>0</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="24"/>
+        <v>8</v>
+      </c>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:5" ht="32.25" customHeight="1">
-      <c r="A16" s="42" t="s">
-        <v>12</v>
+      <c r="A16" s="44" t="s">
+        <v>11</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>0</v>
@@ -1497,21 +1501,21 @@
         <v>1</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="65" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="50" t="s">
-        <v>15</v>
+      <c r="A17" s="45"/>
+      <c r="B17" s="52" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="21">
+        <v>13</v>
+      </c>
+      <c r="D17" s="20">
         <v>231000.00000000003</v>
       </c>
       <c r="E17" s="15">
@@ -1519,12 +1523,12 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="51"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="21">
+        <v>16</v>
+      </c>
+      <c r="D18" s="20">
         <v>258500.00000000003</v>
       </c>
       <c r="E18" s="15">
@@ -1532,12 +1536,12 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="43"/>
-      <c r="B19" s="52"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="21">
+        <v>12</v>
+      </c>
+      <c r="D19" s="20">
         <v>286000</v>
       </c>
       <c r="E19" s="15">
@@ -1545,14 +1549,14 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="43"/>
-      <c r="B20" s="50" t="s">
-        <v>16</v>
+      <c r="A20" s="45"/>
+      <c r="B20" s="52" t="s">
+        <v>15</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="21">
+        <v>13</v>
+      </c>
+      <c r="D20" s="20">
         <v>231000.00000000003</v>
       </c>
       <c r="E20" s="15">
@@ -1560,12 +1564,12 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="43"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="21">
+        <v>16</v>
+      </c>
+      <c r="D21" s="20">
         <v>258500.00000000003</v>
       </c>
       <c r="E21" s="15">
@@ -1573,12 +1577,12 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="43"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="21">
+        <v>12</v>
+      </c>
+      <c r="D22" s="20">
         <v>286000</v>
       </c>
       <c r="E22" s="15">
@@ -1586,14 +1590,14 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A23" s="43"/>
-      <c r="B23" s="53" t="s">
+      <c r="A23" s="45"/>
+      <c r="B23" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>297000</v>
       </c>
       <c r="E23" s="15">
@@ -1601,12 +1605,12 @@
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" ht="39" customHeight="1" thickBot="1">
-      <c r="A24" s="44"/>
-      <c r="B24" s="54"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="22">
+        <v>19</v>
+      </c>
+      <c r="D24" s="21">
         <v>341000</v>
       </c>
       <c r="E24" s="17">
@@ -1621,240 +1625,203 @@
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A26" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="45">
+      <c r="A26" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="47">
         <f>IF(C14=Sheet1!B2,(IFERROR(VLOOKUP('Request Form'!E15,Sheet1!C1:D11,2,0),0)*(C15-1))+(IFERROR(VLOOKUP('Request Form'!E15,Sheet1!C1:E11,3,0),0)),(IFERROR(VLOOKUP('Request Form'!E15,Sheet1!C1:D11,2,0),0)*(C15)))</f>
         <v>0</v>
       </c>
-      <c r="E26" s="46"/>
+      <c r="E26" s="48"/>
     </row>
     <row r="27" spans="1:5" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A27" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
+      <c r="A27" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="59"/>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="60"/>
+      <c r="A28" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="61"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="62"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="64"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A30" s="61"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="62"/>
-    </row>
-    <row r="31" spans="1:5" ht="18.75">
-      <c r="A31" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
+    </row>
+    <row r="31" spans="1:5" ht="19.5" thickBot="1">
+      <c r="A31" s="65"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
     </row>
     <row r="32" spans="1:5" ht="21" customHeight="1">
-      <c r="A32" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="18"/>
-    </row>
-    <row r="33" spans="1:5" ht="21" customHeight="1" thickBot="1">
-      <c r="A33" s="35" t="s">
+      <c r="A32" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="62"/>
+    </row>
+    <row r="33" spans="1:5" ht="21" customHeight="1">
+      <c r="A33" s="67"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="64"/>
+    </row>
+    <row r="34" spans="1:5" ht="21" customHeight="1">
+      <c r="A34" s="67"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="64"/>
+    </row>
+    <row r="35" spans="1:5" ht="21" customHeight="1" thickBot="1">
+      <c r="A35" s="68"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="70"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="18"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="18"/>
-    </row>
-    <row r="34" spans="1:5" ht="21" customHeight="1" thickBot="1">
-      <c r="A34" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="21" customHeight="1" thickBot="1">
-      <c r="A35" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="18"/>
-    </row>
-    <row r="36" spans="1:5" ht="21" customHeight="1" thickBot="1">
-      <c r="A36" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="18"/>
-    </row>
-    <row r="37" spans="1:5" ht="21" customHeight="1" thickBot="1">
-      <c r="A37" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="18"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="18"/>
+      <c r="A38" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="B38" s="19"/>
       <c r="C38" s="18"/>
       <c r="D38" s="19"/>
       <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="18"/>
+      <c r="A39" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="18" t="s">
-        <v>47</v>
-      </c>
+      <c r="A40" s="18"/>
       <c r="B40" s="19"/>
       <c r="C40" s="18"/>
       <c r="D40" s="19"/>
       <c r="E40" s="18"/>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="19"/>
+    <row r="41" spans="1:5" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A41" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="36"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="1:5" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A42" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="36"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="38"/>
       <c r="E42" s="18"/>
     </row>
-    <row r="43" spans="1:5" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A43" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
+    <row r="43" spans="1:5">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="18"/>
     </row>
-    <row r="44" spans="1:5" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A44" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="18"/>
+    <row r="44" spans="1:5">
+      <c r="A44" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="18"/>
+      <c r="A45" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="18"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ioam5iPKY8PF+Ie2BlDAjX3OCHl9BrhpJTkUQDoKbRJUJqUnwaQ/8c1ZqibbK+J+z6PFwsQNUBDUaZKfHhoX+Q==" saltValue="1HRynH/AdECSZIavOdVQ5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="30">
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:E47"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xva+05wGcOAqaNnGPuoAjRI+643FavgEbn4CIAqfYGWM72yCrd83PbAB+uGSVEm2jbRhqhVt0OMApHAuJ78lIQ==" saltValue="v3AmWXUbHDtCASC2b4yfLA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="21">
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A45:E45"/>
     <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A39:E39"/>
     <mergeCell ref="A28:E30"/>
-    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:E35"/>
+    <mergeCell ref="A1:E10"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="A16:A24"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A1:E10"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C35:D35"/>
   </mergeCells>
-  <conditionalFormatting sqref="C12:E13 E15 C33:D37 C43:D44">
+  <conditionalFormatting sqref="C12:E13 E15 C41:D42">
     <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1916,10 +1883,10 @@
   <sheetData>
     <row r="1" spans="2:6">
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="2:6">
@@ -1927,7 +1894,7 @@
         <v>45115</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4">
         <v>231000.00000000003</v>
@@ -1944,7 +1911,7 @@
         <v>45116</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4">
         <v>258500.00000000003</v>
@@ -1961,7 +1928,7 @@
         <v>45117</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4">
         <v>286000</v>
@@ -1975,7 +1942,7 @@
         <v>45118</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="4">
         <v>231000.00000000003</v>
@@ -1989,7 +1956,7 @@
         <v>45119</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4">
         <v>258500.00000000003</v>
@@ -2003,7 +1970,7 @@
         <v>45120</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4">
         <v>286000</v>
@@ -2017,7 +1984,7 @@
         <v>45121</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4">
         <v>297000</v>
@@ -2031,7 +1998,7 @@
         <v>45122</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4">
         <v>341000</v>
@@ -2042,7 +2009,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4">
         <f>D2+198000</f>
@@ -2055,7 +2022,7 @@
     </row>
     <row r="11" spans="2:6">
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4">
         <f>D10</f>
@@ -2067,7 +2034,7 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="C15" s="23"/>
+      <c r="C15" s="22"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="cgFY0yZ5/ryGnKvRJ2qOamE9UBUns7p2l6G7mfVxCTxm6q0URzs6rkMgmkniyjKhzWuL+feIgS7es/Cg+Wtyyw==" saltValue="Knc1RK8OUKjJPy4Bpp8k8Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>